<commit_message>
Adding minimum OA/AO ratios to the extractors
</commit_message>
<xml_diff>
--- a/flowsheet_units.xlsx
+++ b/flowsheet_units.xlsx
@@ -854,10 +854,10 @@
         <v>100000</v>
       </c>
       <c r="F15" t="n">
-        <v>9.347996010082952</v>
+        <v>9.340476362773011</v>
       </c>
       <c r="G15" t="n">
-        <v>200.387418723602</v>
+        <v>197.0182712762979</v>
       </c>
     </row>
     <row r="17">
@@ -928,10 +928,10 @@
         <v>100000</v>
       </c>
       <c r="F19" t="n">
-        <v>9.347996010082952</v>
+        <v>9.340476362773011</v>
       </c>
       <c r="G19" t="n">
-        <v>200.387418723602</v>
+        <v>197.0182712762979</v>
       </c>
     </row>
   </sheetData>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>96</t>
         </is>
       </c>
     </row>
@@ -1373,10 +1373,10 @@
         <v>100000</v>
       </c>
       <c r="F36" t="n">
-        <v>9.347996010082952</v>
+        <v>9.340476362773011</v>
       </c>
       <c r="G36" t="n">
-        <v>200.387418723602</v>
+        <v>197.0182712762979</v>
       </c>
     </row>
     <row r="38">
@@ -1447,10 +1447,10 @@
         <v>100000</v>
       </c>
       <c r="F40" t="n">
-        <v>1.554804084648952</v>
+        <v>1.547284437339011</v>
       </c>
       <c r="G40" t="n">
-        <v>47.43952586043418</v>
+        <v>44.07037841313006</v>
       </c>
     </row>
     <row r="41">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.05</t>
+          <t>0.5</t>
         </is>
       </c>
     </row>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>HNO3, H2O, AHA</t>
+          <t>H2O, AHA, HNO3</t>
         </is>
       </c>
     </row>
@@ -1777,10 +1777,10 @@
         <v>100000</v>
       </c>
       <c r="F24" t="n">
-        <v>1.446066894640746</v>
+        <v>5.900175878399724</v>
       </c>
       <c r="G24" t="n">
-        <v>441.3089661219628</v>
+        <v>1293.926768278144</v>
       </c>
     </row>
     <row r="25">
@@ -1806,10 +1806,10 @@
         <v>100000</v>
       </c>
       <c r="F25" t="n">
-        <v>0.07230334473203728</v>
+        <v>2.950087939199862</v>
       </c>
       <c r="G25" t="n">
-        <v>1.350436276201107</v>
+        <v>55.09988211255751</v>
       </c>
     </row>
     <row r="27">
@@ -1880,10 +1880,10 @@
         <v>100000</v>
       </c>
       <c r="F29" t="n">
-        <v>1.443039583245681</v>
+        <v>5.881288806059096</v>
       </c>
       <c r="G29" t="n">
-        <v>439.9320999959801</v>
+        <v>1285.898456825352</v>
       </c>
     </row>
     <row r="30">
@@ -1909,10 +1909,10 @@
         <v>100000</v>
       </c>
       <c r="F30" t="n">
-        <v>0.07533065612710137</v>
+        <v>2.96897501154049</v>
       </c>
       <c r="G30" t="n">
-        <v>2.727302402183777</v>
+        <v>63.12819356535026</v>
       </c>
     </row>
   </sheetData>
@@ -2098,10 +2098,10 @@
         <v>100000</v>
       </c>
       <c r="F15" t="n">
-        <v>0.07533065612710137</v>
+        <v>2.96897501154049</v>
       </c>
       <c r="G15" t="n">
-        <v>2.727302402183777</v>
+        <v>63.12819356535026</v>
       </c>
     </row>
     <row r="17">
@@ -2172,10 +2172,10 @@
         <v>100000</v>
       </c>
       <c r="F19" t="n">
-        <v>0.07533065612710137</v>
+        <v>2.96897501154049</v>
       </c>
       <c r="G19" t="n">
-        <v>2.727302402183777</v>
+        <v>63.12819356535026</v>
       </c>
     </row>
   </sheetData>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.8733409324271144</t>
+          <t>101.30103657546921</t>
         </is>
       </c>
     </row>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0.8733409324271144</t>
+          <t>101.30103657546921</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>64</t>
         </is>
       </c>
     </row>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0.000325690742036204</t>
+          <t>0.013288684410810188</t>
         </is>
       </c>
     </row>
@@ -2473,7 +2473,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>H2O:0.05; HNO3:0.0005139034985386212</t>
+          <t>H2O:0.4365332828951147; HNO3:0.010630947528648151</t>
         </is>
       </c>
     </row>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>0.35176003846031084</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>H2O:0.021326272505928667; HNO3:0.00013747798553378674</t>
+          <t>H2O:2.4736886030723166; HNO3:0.015946421292972225</t>
         </is>
       </c>
     </row>
@@ -2617,10 +2617,10 @@
         <v>100000</v>
       </c>
       <c r="F36" t="n">
-        <v>0.07533065612710137</v>
+        <v>2.96897501154049</v>
       </c>
       <c r="G36" t="n">
-        <v>2.727302402183777</v>
+        <v>63.12819356535026</v>
       </c>
     </row>
     <row r="38">
@@ -2691,10 +2691,10 @@
         <v>100000</v>
       </c>
       <c r="F40" t="n">
-        <v>0.05402975100665702</v>
+        <v>0.4859843293806062</v>
       </c>
       <c r="G40" t="n">
-        <v>2.336723906987963</v>
+        <v>17.65278531954788</v>
       </c>
     </row>
     <row r="41">
@@ -2720,10 +2720,10 @@
         <v>100000</v>
       </c>
       <c r="F41" t="n">
-        <v>0.02146375049146245</v>
+        <v>2.489635024365289</v>
       </c>
       <c r="G41" t="n">
-        <v>0.3928555620187599</v>
+        <v>45.56831608286056</v>
       </c>
     </row>
   </sheetData>
@@ -2930,10 +2930,10 @@
         <v>100000</v>
       </c>
       <c r="F15" t="n">
-        <v>0.02146375049146245</v>
+        <v>2.489635024365289</v>
       </c>
       <c r="G15" t="n">
-        <v>0.3928555620187599</v>
+        <v>45.56831608286056</v>
       </c>
     </row>
     <row r="17">
@@ -3004,10 +3004,10 @@
         <v>100000</v>
       </c>
       <c r="F19" t="n">
-        <v>7.814655675925462</v>
+        <v>10.28282694979929</v>
       </c>
       <c r="G19" t="n">
-        <v>153.3407484251866</v>
+        <v>198.5162089460284</v>
       </c>
     </row>
   </sheetData>
@@ -3193,10 +3193,10 @@
         <v>100000</v>
       </c>
       <c r="F15" t="n">
-        <v>1.443039583245681</v>
+        <v>5.881288806059096</v>
       </c>
       <c r="G15" t="n">
-        <v>439.9320999959801</v>
+        <v>1285.898456825352</v>
       </c>
     </row>
     <row r="17">
@@ -3267,10 +3267,10 @@
         <v>100000</v>
       </c>
       <c r="F19" t="n">
-        <v>1.443039583245681</v>
+        <v>5.881288806059096</v>
       </c>
       <c r="G19" t="n">
-        <v>439.9320999959801</v>
+        <v>1285.898456825352</v>
       </c>
     </row>
   </sheetData>
@@ -3412,7 +3412,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.6233797469117313</t>
+          <t>0.6233797469117311</t>
         </is>
       </c>
     </row>
@@ -3560,10 +3560,10 @@
         <v>100000</v>
       </c>
       <c r="F24" t="n">
-        <v>1.443039583245681</v>
+        <v>5.881288806059096</v>
       </c>
       <c r="G24" t="n">
-        <v>439.9320999959801</v>
+        <v>1285.898456825352</v>
       </c>
     </row>
     <row r="25">
@@ -3589,10 +3589,10 @@
         <v>100000</v>
       </c>
       <c r="F25" t="n">
-        <v>0.8995616501873031</v>
+        <v>3.666276327435916</v>
       </c>
       <c r="G25" t="n">
-        <v>16.21289638498435</v>
+        <v>66.0776926218041</v>
       </c>
     </row>
     <row r="27">
@@ -3663,10 +3663,10 @@
         <v>100000</v>
       </c>
       <c r="F29" t="n">
-        <v>0.6342004218000266</v>
+        <v>5.080788952460686</v>
       </c>
       <c r="G29" t="n">
-        <v>121.2885419146805</v>
+        <v>970.5369683388589</v>
       </c>
     </row>
     <row r="30">
@@ -3692,10 +3692,10 @@
         <v>100000</v>
       </c>
       <c r="F30" t="n">
-        <v>1.708400811632958</v>
+        <v>4.466776181034326</v>
       </c>
       <c r="G30" t="n">
-        <v>334.856454466284</v>
+        <v>381.4391811082967</v>
       </c>
     </row>
   </sheetData>
@@ -3881,10 +3881,10 @@
         <v>100000</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6342004218000266</v>
+        <v>5.080788952460686</v>
       </c>
       <c r="G15" t="n">
-        <v>121.2885419146805</v>
+        <v>970.5369683388589</v>
       </c>
     </row>
     <row r="17">
@@ -3955,10 +3955,10 @@
         <v>100000</v>
       </c>
       <c r="F19" t="n">
-        <v>0.6342004218000266</v>
+        <v>5.080788952460686</v>
       </c>
       <c r="G19" t="n">
-        <v>121.2885419146805</v>
+        <v>970.5369683388589</v>
       </c>
     </row>
   </sheetData>
@@ -4148,10 +4148,10 @@
         <v>100000</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6342004218000266</v>
+        <v>5.080788952460686</v>
       </c>
       <c r="G15" t="n">
-        <v>121.2885419146805</v>
+        <v>970.5369683388589</v>
       </c>
     </row>
     <row r="17">
@@ -4222,10 +4222,10 @@
         <v>100000</v>
       </c>
       <c r="F19" t="n">
-        <v>0.03171002109000133</v>
+        <v>0.2540394476230343</v>
       </c>
       <c r="G19" t="n">
-        <v>6.064427095734027</v>
+        <v>48.52684841694294</v>
       </c>
     </row>
     <row r="20">
@@ -4251,10 +4251,10 @@
         <v>100000</v>
       </c>
       <c r="F20" t="n">
-        <v>0.6024904007100251</v>
+        <v>4.826749504837651</v>
       </c>
       <c r="G20" t="n">
-        <v>115.2241148189465</v>
+        <v>922.0101199219158</v>
       </c>
     </row>
   </sheetData>
@@ -6294,10 +6294,10 @@
         <v>100000</v>
       </c>
       <c r="F14" t="n">
-        <v>0.6024904007100251</v>
+        <v>4.826749504837651</v>
       </c>
       <c r="G14" t="n">
-        <v>115.2241148189465</v>
+        <v>922.0101199219158</v>
       </c>
     </row>
     <row r="15">
@@ -6323,10 +6323,10 @@
         <v>100000</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0316673951310102</v>
+        <v>0.2539976294970997</v>
       </c>
       <c r="G15" t="n">
-        <v>6.048127100517057</v>
+        <v>48.51077709654021</v>
       </c>
     </row>
     <row r="17">
@@ -6397,10 +6397,10 @@
         <v>100000</v>
       </c>
       <c r="F19" t="n">
-        <v>0.6341577961036978</v>
+        <v>5.080747132552736</v>
       </c>
       <c r="G19" t="n">
-        <v>121.2722419691607</v>
+        <v>970.5208966780378</v>
       </c>
     </row>
   </sheetData>
@@ -6590,7 +6590,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0.06241768887837913</t>
+          <t>0.5000782072503869</t>
         </is>
       </c>
     </row>
@@ -6602,7 +6602,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>I_aq, Eu(NO3)3, H2O, Sm(NO3)3, CsNO3, HNO3, Gd(NO3)3, Sr(NO3)2, Nd(NO3)3</t>
+          <t>CsNO3, H2O, Sr(NO3)2, I_aq, Nd(NO3)3, HNO3, Sm(NO3)3, Gd(NO3)3, Eu(NO3)3</t>
         </is>
       </c>
     </row>
@@ -6727,10 +6727,10 @@
         <v>100000</v>
       </c>
       <c r="F25" t="n">
-        <v>0.6341577961036978</v>
+        <v>5.080747132552736</v>
       </c>
       <c r="G25" t="n">
-        <v>121.2722419691607</v>
+        <v>970.5208966780378</v>
       </c>
     </row>
     <row r="27">
@@ -6801,10 +6801,10 @@
         <v>100000</v>
       </c>
       <c r="F29" t="n">
-        <v>1.446066894640746</v>
+        <v>5.900175878399724</v>
       </c>
       <c r="G29" t="n">
-        <v>441.3089661219628</v>
+        <v>1293.926768278144</v>
       </c>
     </row>
     <row r="30">
@@ -6830,10 +6830,10 @@
         <v>100000</v>
       </c>
       <c r="F30" t="n">
-        <v>9.347996010082952</v>
+        <v>9.340476362773011</v>
       </c>
       <c r="G30" t="n">
-        <v>200.387418723602</v>
+        <v>197.0182712762979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renaming placeholder stream names
</commit_message>
<xml_diff>
--- a/flowsheet_units.xlsx
+++ b/flowsheet_units.xlsx
@@ -16,20 +16,20 @@
     <sheet name="M114_OrgFeedMixer" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="X101_TBP_Extraction" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="CF101_Coalescer_X101_to_E101" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="HX__F101-T" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="PC__F101-p" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="HX__F53-T" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="PC__F53-p" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="E101_Evaporator" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="X102_AHA_Strip" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="CF102_Coalescer_X102_to_E102" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="HX__F102-T" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="PC__F102-p" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="HX__F55-T" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="PC__F55-p" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="E102_Evaporator" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="M201_EvapOverheadMixer" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="HX__F10-T" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="HX__F11-T" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="X103_Final_Strip" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="CF103_Coalescer_X103_to_E103" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="HX__F112-T" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="HX__F57-T" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="E103_Evaporator100C" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="HX__F24-T" sheetId="25" state="visible" r:id="rId25"/>
     <sheet name="R201_UO3_Calciner" sheetId="26" state="visible" r:id="rId26"/>
@@ -766,7 +766,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>HX__F101-T</t>
+          <t>HX__F53-T</t>
         </is>
       </c>
     </row>
@@ -907,7 +907,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>F101</t>
+          <t>F53</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -981,7 +981,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>F101-T</t>
+          <t>F53-T</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>PC__F101-p</t>
+          <t>PC__F53-p</t>
         </is>
       </c>
     </row>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>F101-T</t>
+          <t>F53-T</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>F101-p</t>
+          <t>F53-p</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>F101-p</t>
+          <t>F53-p</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>AHA, HNO3, H2O</t>
+          <t>AHA, H2O, HNO3</t>
         </is>
       </c>
     </row>
@@ -2696,7 +2696,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>F102</t>
+          <t>F55</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2725,7 +2725,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>F106</t>
+          <t>F56</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2773,7 +2773,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>HX__F102-T</t>
+          <t>HX__F55-T</t>
         </is>
       </c>
     </row>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>F102</t>
+          <t>F55</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2988,7 +2988,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>F102-T</t>
+          <t>F55-T</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -3036,7 +3036,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>PC__F102-p</t>
+          <t>PC__F55-p</t>
         </is>
       </c>
     </row>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>F102-T</t>
+          <t>F55-T</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -3251,7 +3251,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>F102-p</t>
+          <t>F55-p</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -3720,7 +3720,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>F102-p</t>
+          <t>F55-p</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -5814,7 +5814,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>F112</t>
+          <t>F57</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -5843,7 +5843,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>F113</t>
+          <t>F58</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -5891,7 +5891,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>HX__F112-T</t>
+          <t>HX__F57-T</t>
         </is>
       </c>
     </row>
@@ -6032,7 +6032,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>F112</t>
+          <t>F57</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -6106,7 +6106,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>F112-T</t>
+          <t>F57-T</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -6347,7 +6347,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>F112-T</t>
+          <t>F57-T</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -11405,7 +11405,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>F138</t>
+          <t>F59</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -14173,7 +14173,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>F145</t>
+          <t>F60</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -16168,7 +16168,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>F105</t>
+          <t>F54</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -16197,7 +16197,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>F106</t>
+          <t>F56</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -16226,7 +16226,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>F113</t>
+          <t>F58</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -16300,7 +16300,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>F107</t>
+          <t>F61</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -16510,7 +16510,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>F107</t>
+          <t>F61</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -16584,7 +16584,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>F13_mix</t>
+          <t>F62</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -16773,7 +16773,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>F13_mix</t>
+          <t>F62</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -17934,7 +17934,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Sr(NO3)2, CsNO3, H2O, HNO3, I_aq, Sm(NO3)3, Eu(NO3)3, Gd(NO3)3, Nd(NO3)3</t>
+          <t>Sm(NO3)3, Sr(NO3)2, CsNO3, HNO3, I_aq, Gd(NO3)3, H2O, Eu(NO3)3, Nd(NO3)3</t>
         </is>
       </c>
     </row>
@@ -18594,7 +18594,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>F101</t>
+          <t>F53</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -18623,7 +18623,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>F105</t>
+          <t>F54</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">

</xml_diff>

<commit_message>
Fixing TSA Iodine system
</commit_message>
<xml_diff>
--- a/flowsheet_units.xlsx
+++ b/flowsheet_units.xlsx
@@ -1235,7 +1235,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>H2O, Gd(NO3)3, I_aq, CsNO3, HNO3, Sm(NO3)3, Sr(NO3)2, Nd(NO3)3, Eu(NO3)3</t>
+          <t>HNO3, Gd(NO3)3, H2O, Eu(NO3)3, Nd(NO3)3, I_aq, Sr(NO3)2, CsNO3, Sm(NO3)3</t>
         </is>
       </c>
     </row>
@@ -3242,7 +3242,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>H2O, AHA, HNO3</t>
+          <t>HNO3, H2O, AHA</t>
         </is>
       </c>
     </row>
@@ -16793,7 +16793,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16897,7 +16897,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.00108381924</t>
         </is>
       </c>
     </row>
@@ -16976,290 +16976,310 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>iodine_name</t>
+          <t>captured_cycle_mol</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>I_g</t>
+          <t>15.606997056</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>loading_cycle_mol</t>
+          <t>iodine_name</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>15.606997056</t>
+          <t>I_g</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>mode</t>
+          <t>loading_cycle_mol</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>adsorb</t>
+          <t>15.606997056</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>print_diagnostics</t>
+          <t>mode</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>adsorb</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>regen_yI2_max</t>
+          <t>print_diagnostics</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0.1</t>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>t_ads_s</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>28800.0</t>
-        </is>
-      </c>
+          <t>regen_source</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>t_regen_s</t>
+          <t>regen_yI2_max</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>14400.0</t>
+          <t>0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>t_ads_s</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>28800.0</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Inlets</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>port</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>stream</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>phase</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>T [K]</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>p [Pa]</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>F_total [mol/s]</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>m_dot [g/s]</t>
+          <t>t_regen_s</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>14400.0</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>gas_in</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>F49A</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>298.15</v>
-      </c>
-      <c r="E28" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F28" t="n">
-        <v>1.847803820760401</v>
-      </c>
-      <c r="G28" t="n">
-        <v>53.72283748547709</v>
-      </c>
+          <t>Inlets</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>regen_in</t>
+          <t>port</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>F52A</t>
+          <t>stream</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>phase</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>T [K]</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>p [Pa]</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>F_total [mol/s]</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>m_dot [g/s]</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>gas_in</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>F49A</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
           <t>G</t>
         </is>
       </c>
-      <c r="D29" t="n">
-        <v>423.15</v>
-      </c>
-      <c r="E29" t="n">
+      <c r="D30" t="n">
+        <v>298.15</v>
+      </c>
+      <c r="E30" t="n">
         <v>100000</v>
       </c>
-      <c r="F29" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0</v>
+      <c r="F30" t="n">
+        <v>1.847803820760401</v>
+      </c>
+      <c r="G30" t="n">
+        <v>53.72283748547709</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Outlets</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>port</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>stream</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>phase</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>T [K]</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>p [Pa]</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>F_total [mol/s]</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>m_dot [g/s]</t>
-        </is>
+          <t>regen_in</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>F52A</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>423.15</v>
+      </c>
+      <c r="E31" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>gas_out</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>F50A</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>298.15</v>
-      </c>
-      <c r="E33" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F33" t="n">
-        <v>1.847261911140401</v>
-      </c>
-      <c r="G33" t="n">
-        <v>53.58302480351708</v>
-      </c>
+          <t>Outlets</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>port</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>stream</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>phase</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>T [K]</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>p [Pa]</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>F_total [mol/s]</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>m_dot [g/s]</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>gas_out</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>F50A</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>298.15</v>
+      </c>
+      <c r="E35" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1.847261911140401</v>
+      </c>
+      <c r="G35" t="n">
+        <v>53.58302480351708</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>regen_out</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B36" t="inlineStr">
         <is>
           <t>F51A</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="D36" t="n">
         <v>298.15</v>
       </c>
-      <c r="E34" t="n">
+      <c r="E36" t="n">
         <v>100000</v>
       </c>
-      <c r="F34" t="n">
+      <c r="F36" t="n">
         <v>0</v>
       </c>
-      <c r="G34" t="n">
+      <c r="G36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17274,7 +17294,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17457,290 +17477,314 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>iodine_name</t>
+          <t>captured_cycle_mol</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>I_g</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>loading_cycle_mol</t>
+          <t>iodine_name</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>I_g</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>mode</t>
+          <t>loading_cycle_mol</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>regen</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>print_diagnostics</t>
+          <t>mode</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>regen</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>regen_yI2_max</t>
+          <t>print_diagnostics</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0.1</t>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>t_ads_s</t>
+          <t>regen_source</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>28800.0</t>
+          <t>&lt;process_sim.unitops.TSA.IdealTSAColumnEMM17 object at 0x0000018955AC5160&gt;</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>t_regen_s</t>
+          <t>regen_yI2_max</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>14400.0</t>
+          <t>0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>t_ads_s</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>28800.0</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Inlets</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>port</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>stream</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>phase</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>T [K]</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>p [Pa]</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>F_total [mol/s]</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>m_dot [g/s]</t>
+          <t>t_regen_s</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>14400.0</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>gas_in</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>F49B</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>298.15</v>
-      </c>
-      <c r="E28" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0</v>
-      </c>
+          <t>Inlets</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>regen_in</t>
+          <t>port</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>F52B</t>
+          <t>stream</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>phase</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>T [K]</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>p [Pa]</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>F_total [mol/s]</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>m_dot [g/s]</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>gas_in</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>F49B</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
           <t>G</t>
         </is>
       </c>
-      <c r="D29" t="n">
-        <v>423.15</v>
-      </c>
-      <c r="E29" t="n">
+      <c r="D30" t="n">
+        <v>298.15</v>
+      </c>
+      <c r="E30" t="n">
         <v>100000</v>
       </c>
-      <c r="F29" t="n">
-        <v>0.0108381924</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0.5610452723848225</v>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Outlets</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>port</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>stream</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>phase</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>T [K]</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>p [Pa]</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>F_total [mol/s]</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>m_dot [g/s]</t>
-        </is>
+          <t>regen_in</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>F52B</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>423.15</v>
+      </c>
+      <c r="E31" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.009754373160000001</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.2814199084648225</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>gas_out</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>F50B</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="D33" t="n">
-        <v>298.15</v>
-      </c>
-      <c r="E33" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0</v>
-      </c>
+          <t>Outlets</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>port</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>stream</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>phase</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>T [K]</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>p [Pa]</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>F_total [mol/s]</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>m_dot [g/s]</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>gas_out</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>F50B</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>298.15</v>
+      </c>
+      <c r="E35" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>regen_out</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B36" t="inlineStr">
         <is>
           <t>F51B</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="D34" t="n">
+      <c r="D36" t="n">
         <v>298.15</v>
       </c>
-      <c r="E34" t="n">
+      <c r="E36" t="n">
         <v>100000</v>
       </c>
-      <c r="F34" t="n">
+      <c r="F36" t="n">
         <v>0.0108381924</v>
       </c>
-      <c r="G34" t="n">
+      <c r="G36" t="n">
         <v>0.5610452723848225</v>
       </c>
     </row>

</xml_diff>